<commit_message>
update format for output
</commit_message>
<xml_diff>
--- a/path2shock_calculation/output/path2shock_Base.xlsx
+++ b/path2shock_calculation/output/path2shock_Base.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,8 +466,10 @@
           <t>MMM1</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0.2</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20.0 %</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr"/>
     </row>
@@ -482,8 +484,10 @@
           <t>MMM2</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>0.04347826086956519</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4.3 %</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr"/>
     </row>
@@ -498,8 +502,10 @@
           <t>MMM3</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0.02439024390243905</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2.4 %</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr"/>
     </row>
@@ -514,8 +520,10 @@
           <t>MMM4</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.01694915254237284</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.7 %</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr"/>
     </row>
@@ -530,8 +538,10 @@
           <t>MMM5</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0.01298701298701288</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.3 %</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr"/>
     </row>
@@ -546,8 +556,10 @@
           <t>MMM6</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0.01052631578947372</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.1 %</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
@@ -562,8 +574,10 @@
           <t>MMM7</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>0.008849557522123908</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0.9 %</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr"/>
     </row>
@@ -578,8 +592,10 @@
           <t>MMM8</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0.007633587786259444</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.8 %</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr"/>
     </row>
@@ -594,8 +610,10 @@
           <t>MMM9</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>0.006711409395973256</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.7 %</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr"/>
     </row>
@@ -610,8 +628,10 @@
           <t>MMM10</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.07784431137724557</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>7.8 %</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr"/>
     </row>
@@ -626,11 +646,15 @@
           <t>MMM11</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>13</v>
-      </c>
-      <c r="D12" t="n">
-        <v>198</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>13% max</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>(+198 ppts)</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -644,11 +668,15 @@
           <t>MMM12</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>13</v>
-      </c>
-      <c r="D13" t="n">
-        <v>216</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>13 peak</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>(+216 ppts)</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -662,11 +690,15 @@
           <t>MMM13</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>13</v>
-      </c>
-      <c r="D14" t="n">
-        <v>234</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>13% peak</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>(+23400 bps)</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -680,288 +712,144 @@
           <t>MMM14</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>13</v>
-      </c>
-      <c r="D15" t="n">
-        <v>252</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>13% peak</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>(+25200 bps)</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>M15</t>
+          <t>M20</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MMM15</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>13</v>
-      </c>
-      <c r="D16" t="n">
-        <v>270</v>
+          <t>MMM20</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1.1 %</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1.2 %</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>M16</t>
+          <t>M21</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MMM16</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>13</v>
-      </c>
-      <c r="D17" t="n">
-        <v>288</v>
+          <t>MMM21</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>13% peak</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>(+37800 bps)</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M17</t>
+          <t>M22</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MMM17</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>13</v>
-      </c>
-      <c r="D18" t="n">
-        <v>306</v>
+          <t>MMM22</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>13% peak</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>(+39600 bps)</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M18</t>
+          <t>M23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MMM18</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>13</v>
-      </c>
-      <c r="D19" t="n">
-        <v>324</v>
+          <t>MMM23</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>13% peak</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>(+41400 bps)</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M19</t>
+          <t>M24</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MMM19</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>13</v>
-      </c>
-      <c r="D20" t="n">
-        <v>342</v>
-      </c>
+          <t>MMM24</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.2 %</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>M20</t>
+          <t>M25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MMM20</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0.01118870236745795</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.01157730348796671</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>M21</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>MMM21</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>M22</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>MMM22</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" t="n">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>M23</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>MMM23</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" t="n">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>M24</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>MMM24</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0.002386634844868674</v>
-      </c>
-      <c r="D25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>M25</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
           <t>MMM25</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" t="n">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>M26</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>MMM26</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>0.00219780219780219</v>
-      </c>
-      <c r="D27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>M27</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>MMM27</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>0.002114164904862603</v>
-      </c>
-      <c r="D28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>M28</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>MMM28</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>0.002036659877800329</v>
-      </c>
-      <c r="D29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>M29</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>MMM29</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>0.001964636542239662</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>M30</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>MMM30</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>0.00189753320683117</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>13% peak</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>(+45000 bps)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update output format to keep numeric output
</commit_message>
<xml_diff>
--- a/path2shock_calculation/output/path2shock_Base.xlsx
+++ b/path2shock_calculation/output/path2shock_Base.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>extreme_level</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>shock_raw</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>extreme_level_raw</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,6 +482,10 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -490,6 +504,10 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.04347826086956519</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -508,6 +526,10 @@
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.02439024390243905</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -526,6 +548,10 @@
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.01694915254237284</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -544,6 +570,10 @@
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.01298701298701288</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -562,6 +592,10 @@
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.01052631578947372</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -580,6 +614,10 @@
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0.008849557522123908</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -598,6 +636,10 @@
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.007633587786259444</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -616,6 +658,10 @@
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>0.006711409395973256</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -634,6 +680,10 @@
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>0.07784431137724557</v>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -656,6 +706,12 @@
           <t>(+198 ppts)</t>
         </is>
       </c>
+      <c r="E12" t="n">
+        <v>13</v>
+      </c>
+      <c r="F12" t="n">
+        <v>198</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -678,6 +734,12 @@
           <t>(+216 ppts)</t>
         </is>
       </c>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
+      <c r="F13" t="n">
+        <v>216</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -700,6 +762,12 @@
           <t>(+23400 bps)</t>
         </is>
       </c>
+      <c r="E14" t="n">
+        <v>13</v>
+      </c>
+      <c r="F14" t="n">
+        <v>234</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -722,6 +790,12 @@
           <t>(+25200 bps)</t>
         </is>
       </c>
+      <c r="E15" t="n">
+        <v>13</v>
+      </c>
+      <c r="F15" t="n">
+        <v>252</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -744,6 +818,12 @@
           <t>1.2 %</t>
         </is>
       </c>
+      <c r="E16" t="n">
+        <v>0.01118870236745795</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.01157730348796671</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -766,6 +846,12 @@
           <t>(+37800 bps)</t>
         </is>
       </c>
+      <c r="E17" t="n">
+        <v>13</v>
+      </c>
+      <c r="F17" t="n">
+        <v>378</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -788,6 +874,12 @@
           <t>(+39600 bps)</t>
         </is>
       </c>
+      <c r="E18" t="n">
+        <v>13</v>
+      </c>
+      <c r="F18" t="n">
+        <v>396</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -810,6 +902,12 @@
           <t>(+41400 bps)</t>
         </is>
       </c>
+      <c r="E19" t="n">
+        <v>13</v>
+      </c>
+      <c r="F19" t="n">
+        <v>414</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -828,6 +926,10 @@
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>0.002386634844868674</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -849,6 +951,12 @@
         <is>
           <t>(+45000 bps)</t>
         </is>
+      </c>
+      <c r="E21" t="n">
+        <v>13</v>
+      </c>
+      <c r="F21" t="n">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>